<commit_message>
Implemented getting feign relationship between microservices. Changed measure code, so it reads data from own parser.
</commit_message>
<xml_diff>
--- a/data/backend/backend_structure.xlsx
+++ b/data/backend/backend_structure.xlsx
@@ -6,14 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="data1" r:id="rId3" sheetId="1"/>
-    <sheet name="data2" r:id="rId4" sheetId="2"/>
+    <sheet name="feignRelations" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Source Service Name</t>
   </si>
@@ -24,16 +23,13 @@
     <t>Source Method Signature</t>
   </si>
   <si>
-    <t>Target Microservice Name</t>
+    <t>Target Service Name</t>
   </si>
   <si>
     <t>Target Interface Name</t>
   </si>
   <si>
     <t>Target Operation Signature</t>
-  </si>
-  <si>
-    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -68,79 +64,40 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>